<commit_message>
EPBDS-2771 Add a test for ={<formula>} expression in SimpleRules
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-2771_formula_in_braces.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-2771_formula_in_braces.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Datatype Foo &lt;String&gt;</t>
   </si>
@@ -49,9 +49,6 @@
     <t>COVCODE</t>
   </si>
   <si>
-    <t>SimpleRules Foo[] tte(boolean test)</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -68,6 +65,27 @@
   </si>
   <si>
     <t>= {fooTable2;}</t>
+  </si>
+  <si>
+    <t>Test expr</t>
+  </si>
+  <si>
+    <t>SimpleRules Foo[] expr(boolean in)</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>1,3,5</t>
+  </si>
+  <si>
+    <t>2,4,6</t>
   </si>
 </sst>
 </file>
@@ -196,13 +214,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I18"/>
+  <dimension ref="B4:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -520,42 +538,42 @@
     <col min="8" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:13">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:13">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:13">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:13">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:13">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:13">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:13">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:13">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -563,69 +581,96 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:13">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1">
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="16.5" thickTop="1" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="16.5" thickTop="1" thickBot="1">
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" thickTop="1"/>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H14:I14"/>

</xml_diff>